<commit_message>
Refactor: se actualiza inventario , presentacion 2 trimestre , sentencias ffl y presupuesto
</commit_message>
<xml_diff>
--- a/3.Diseño/Informe_de_costos/Presupuesto.xlsx
+++ b/3.Diseño/Informe_de_costos/Presupuesto.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F\Desktop\QrLean\2.Analisis\Diagrama de gantt - Presupuesto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F\Desktop\QrLean\3.Diseño\Informe_de_costos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1566126-9BBC-498F-8368-BCEA528233EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065C465A-FB38-4123-9F16-AE82808F5A77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="20610" windowHeight="10980" xr2:uid="{634AC136-4E74-477E-8CDE-B990AACE1D10}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>12/24/2021</t>
   </si>
   <si>
-    <t>Presupuesto proyecto</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -436,6 +433,9 @@
   <si>
     <t>Libre office</t>
   </si>
+  <si>
+    <t>Presupuesto proyecto</t>
+  </si>
 </sst>
 </file>
 
@@ -445,7 +445,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-240A]\ * #,##0.00_);_([$$-240A]\ * \(#,##0.00\);_([$$-240A]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,6 +484,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -602,7 +610,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -716,6 +724,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1477,8 +1488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3951A6DF-4FCE-4AD0-9879-7A933B15F254}">
   <dimension ref="B1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1507,7 @@
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="33.75" x14ac:dyDescent="0.65">
       <c r="B2" s="27" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -1509,7 +1520,7 @@
       <c r="K2" s="52"/>
     </row>
     <row r="3" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="19"/>
+      <c r="B3" s="58"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -1534,13 +1545,13 @@
     </row>
     <row r="5" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>13</v>
-      </c>
       <c r="D5" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="48">
         <v>8</v>
@@ -1560,20 +1571,20 @@
         <v>1</v>
       </c>
       <c r="D6" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -1584,10 +1595,10 @@
         <v>3</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -1606,7 +1617,7 @@
       <c r="B8" s="19"/>
       <c r="C8" s="14"/>
       <c r="D8" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E8" s="50">
         <v>3725.81756068</v>
@@ -1620,28 +1631,28 @@
     </row>
     <row r="9" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
       <c r="F9" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="H9" s="24" t="s">
         <v>8</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>9</v>
       </c>
       <c r="I9" s="24"/>
       <c r="J9" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="25" t="s">
         <v>10</v>
-      </c>
-      <c r="K9" s="25" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -1649,7 +1660,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1662,24 +1673,24 @@
     </row>
     <row r="11" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>15</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>16</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H11" s="14">
         <v>18</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J11" s="20">
         <f>Software!I7</f>
@@ -1692,24 +1703,24 @@
     </row>
     <row r="12" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B12" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>18</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>19</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H12" s="14">
         <v>18</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J12" s="20">
         <f>Software!I8</f>
@@ -1722,24 +1733,24 @@
     </row>
     <row r="13" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H13" s="14">
         <v>18</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J13" s="20">
         <f>Software!I9</f>
@@ -1752,24 +1763,24 @@
     </row>
     <row r="14" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H14" s="14">
         <v>2</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J14" s="20">
         <f>Software!I10</f>
@@ -1782,24 +1793,24 @@
     </row>
     <row r="15" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J15" s="20">
         <v>0</v>
@@ -1810,24 +1821,24 @@
     </row>
     <row r="16" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J16" s="20">
         <v>0</v>
@@ -1838,24 +1849,24 @@
     </row>
     <row r="17" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>98</v>
-      </c>
       <c r="H17" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J17" s="20">
         <v>0</v>
@@ -1866,24 +1877,24 @@
     </row>
     <row r="18" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J18" s="20">
         <v>0</v>
@@ -1894,24 +1905,24 @@
     </row>
     <row r="19" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J19" s="20">
         <v>0</v>
@@ -1922,24 +1933,24 @@
     </row>
     <row r="20" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B20" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J20" s="20">
         <v>0</v>
@@ -1950,24 +1961,24 @@
     </row>
     <row r="21" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B21" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J21" s="20">
         <v>0</v>
@@ -1986,7 +1997,7 @@
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K22" s="17">
         <f>K11+K12+K13+K14</f>
@@ -2003,7 +2014,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K23" s="17">
         <f>Software!K18</f>
@@ -2015,7 +2026,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -2028,24 +2039,24 @@
     </row>
     <row r="25" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H25" s="14">
         <v>3456</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J25" s="20">
         <f>Personal!J7</f>
@@ -2058,24 +2069,24 @@
     </row>
     <row r="26" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B26" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
       <c r="F26" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H26" s="14">
         <v>3456</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J26" s="20">
         <f>Personal!J8</f>
@@ -2088,24 +2099,24 @@
     </row>
     <row r="27" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B27" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
       <c r="F27" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H27" s="14">
         <v>3456</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J27" s="20">
         <f>Personal!J9</f>
@@ -2118,24 +2129,24 @@
     </row>
     <row r="28" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>29</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>30</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
       <c r="F28" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H28" s="14">
         <v>3456</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J28" s="20">
         <f>Personal!J10</f>
@@ -2156,7 +2167,7 @@
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K29" s="17">
         <f>K28+K27+K26+K25</f>
@@ -2173,7 +2184,7 @@
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
       <c r="J30" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K30" s="17">
         <f>Personal!Q11</f>
@@ -2185,7 +2196,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -2198,24 +2209,24 @@
     </row>
     <row r="32" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B32" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="21"/>
       <c r="F32" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H32" s="14">
         <v>4</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J32" s="22">
         <f>'Hardware-equipos'!G7</f>
@@ -2228,24 +2239,24 @@
     </row>
     <row r="33" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="21"/>
       <c r="F33" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H33" s="14">
         <v>4</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J33" s="22">
         <f>'Hardware-equipos'!G8</f>
@@ -2258,24 +2269,24 @@
     </row>
     <row r="34" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B34" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="21"/>
       <c r="F34" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H34" s="14">
         <v>4</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J34" s="22">
         <f>'Hardware-equipos'!G9</f>
@@ -2296,7 +2307,7 @@
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
       <c r="J35" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K35" s="23">
         <f>K34+K33+K32</f>
@@ -2313,7 +2324,7 @@
       <c r="H36" s="21"/>
       <c r="I36" s="21"/>
       <c r="J36" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K36" s="17">
         <f>'Hardware-equipos'!K10</f>
@@ -2325,7 +2336,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -2338,24 +2349,24 @@
     </row>
     <row r="38" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B38" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="21"/>
       <c r="F38" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H38" s="14">
         <v>18</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J38" s="20">
         <f>Servicios!G7</f>
@@ -2368,24 +2379,24 @@
     </row>
     <row r="39" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B39" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="21"/>
       <c r="F39" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G39" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H39" s="14">
         <v>18</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J39" s="20">
         <f>Servicios!G8</f>
@@ -2398,24 +2409,24 @@
     </row>
     <row r="40" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B40" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="21"/>
       <c r="F40" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H40" s="14">
         <v>18</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J40" s="20">
         <f>Servicios!G9</f>
@@ -2436,7 +2447,7 @@
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
       <c r="J41" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K41" s="23">
         <f>K40+K39+K38</f>
@@ -2453,7 +2464,7 @@
       <c r="H42" s="21"/>
       <c r="I42" s="21"/>
       <c r="J42" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K42" s="17">
         <f>Servicios!I10</f>
@@ -2465,7 +2476,7 @@
         <v>5</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
@@ -2478,24 +2489,24 @@
     </row>
     <row r="44" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B44" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="21"/>
       <c r="F44" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H44" s="14">
         <v>18</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J44" s="20">
         <f>Lugar!G7</f>
@@ -2516,7 +2527,7 @@
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K45" s="23">
         <f>K44</f>
@@ -2533,7 +2544,7 @@
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>
       <c r="J46" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K46" s="17">
         <f>Lugar!I8</f>
@@ -2590,17 +2601,17 @@
       <c r="B2" s="55"/>
       <c r="C2" s="55"/>
       <c r="D2" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="55"/>
       <c r="C3" s="55"/>
       <c r="D3" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2">
         <f>J18</f>
@@ -2611,7 +2622,7 @@
       <c r="B4" s="55"/>
       <c r="C4" s="55"/>
       <c r="D4" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2">
         <f>K18</f>
@@ -2620,32 +2631,32 @@
     </row>
     <row r="6" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="37" t="s">
-        <v>69</v>
-      </c>
       <c r="F6" s="56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="56"/>
       <c r="H6" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K6" s="43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -2653,19 +2664,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>17</v>
       </c>
       <c r="F7" s="14">
         <v>18</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H7" s="20">
         <v>8.99</v>
@@ -2688,19 +2699,19 @@
         <v>2</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="14">
         <v>18</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H8" s="20">
         <v>25</v>
@@ -2723,19 +2734,19 @@
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="14">
         <v>18</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H9" s="20">
         <v>20</v>
@@ -2758,19 +2769,19 @@
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="14">
         <v>2</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H10" s="20">
         <v>14.04</v>
@@ -2793,19 +2804,19 @@
         <v>5</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F11" s="14">
         <v>18</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H11" s="20">
         <v>0</v>
@@ -2825,19 +2836,19 @@
         <v>6</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F12" s="14">
         <v>18</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H12" s="20">
         <v>0</v>
@@ -2857,19 +2868,19 @@
         <v>7</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D13" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>97</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>98</v>
       </c>
       <c r="F13" s="14">
         <v>18</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H13" s="20">
         <v>0</v>
@@ -2889,19 +2900,19 @@
         <v>8</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F14" s="14">
         <v>18</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H14" s="20">
         <v>0</v>
@@ -2921,19 +2932,19 @@
         <v>9</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F15" s="14">
         <v>18</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H15" s="20">
         <v>0</v>
@@ -2953,19 +2964,19 @@
         <v>10</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F16" s="14">
         <v>18</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H16" s="20">
         <v>0</v>
@@ -2985,19 +2996,19 @@
         <v>11</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F17" s="14">
         <v>18</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H17" s="20">
         <v>0</v>
@@ -3014,7 +3025,7 @@
     </row>
     <row r="18" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="57"/>
       <c r="D18" s="57"/>
@@ -3083,17 +3094,17 @@
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2">
         <f>P11</f>
@@ -3104,7 +3115,7 @@
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
       <c r="D4" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2">
         <f>Q11</f>
@@ -3113,50 +3124,50 @@
     </row>
     <row r="6" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="G6" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="H6" s="43" t="s">
+      <c r="J6" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="L6" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="I6" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="J6" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="K6" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="L6" s="43" t="s">
+      <c r="M6" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" s="56" t="s">
         <v>85</v>
-      </c>
-      <c r="M6" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="N6" s="56" t="s">
-        <v>86</v>
       </c>
       <c r="O6" s="56"/>
       <c r="P6" s="37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q6" s="43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
@@ -3164,13 +3175,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="14">
         <v>8</v>
@@ -3204,7 +3215,7 @@
         <v>3456</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P7" s="35">
         <f>N7*J7</f>
@@ -3220,13 +3231,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="14">
         <v>8</v>
@@ -3260,7 +3271,7 @@
         <v>3456</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P8" s="35">
         <f t="shared" ref="P8:P10" si="4">N8*J8</f>
@@ -3276,13 +3287,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="14">
         <v>8</v>
@@ -3316,7 +3327,7 @@
         <v>3456</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P9" s="35">
         <f t="shared" si="4"/>
@@ -3332,13 +3343,13 @@
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="14">
         <v>8</v>
@@ -3372,7 +3383,7 @@
         <v>3456</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P10" s="35">
         <f t="shared" si="4"/>
@@ -3385,7 +3396,7 @@
     </row>
     <row r="11" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="45"/>
       <c r="D11" s="45"/>
@@ -3445,17 +3456,17 @@
       <c r="B2" s="55"/>
       <c r="C2" s="55"/>
       <c r="D2" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="55"/>
       <c r="C3" s="55"/>
       <c r="D3" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2">
         <f>I10</f>
@@ -3466,7 +3477,7 @@
       <c r="B4" s="55"/>
       <c r="C4" s="55"/>
       <c r="D4" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2">
         <f>K10</f>
@@ -3475,32 +3486,32 @@
     </row>
     <row r="6" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="J6" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="J6" s="41" t="s">
-        <v>117</v>
-      </c>
       <c r="K6" s="43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -3508,22 +3519,22 @@
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="14">
         <v>4</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="22">
         <v>2550000</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I7" s="35">
         <f>G7*E7</f>
@@ -3543,22 +3554,22 @@
         <v>2</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="14">
         <v>4</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="20">
         <v>356000</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I8" s="35">
         <f>G8*E8</f>
@@ -3578,22 +3589,22 @@
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>40</v>
       </c>
       <c r="E9" s="14">
         <v>4</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="20">
         <v>200000</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I9" s="35">
         <f>G9*E9</f>
@@ -3610,7 +3621,7 @@
     </row>
     <row r="10" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="57"/>
       <c r="D10" s="57"/>
@@ -3666,17 +3677,17 @@
       <c r="B2" s="55"/>
       <c r="C2" s="55"/>
       <c r="D2" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="55"/>
       <c r="C3" s="55"/>
       <c r="D3" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2">
         <f>H10</f>
@@ -3687,7 +3698,7 @@
       <c r="B4" s="55"/>
       <c r="C4" s="55"/>
       <c r="D4" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2">
         <f>I10</f>
@@ -3696,26 +3707,26 @@
     </row>
     <row r="6" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="37" t="s">
-        <v>65</v>
-      </c>
       <c r="I6" s="43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -3723,16 +3734,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="14">
         <v>18</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" s="20">
         <v>80000</v>
@@ -3751,16 +3762,16 @@
         <v>2</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="14">
         <v>18</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" s="20">
         <v>40000</v>
@@ -3779,16 +3790,16 @@
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>48</v>
       </c>
       <c r="E9" s="14">
         <v>18</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9" s="20">
         <v>40000</v>
@@ -3804,7 +3815,7 @@
     </row>
     <row r="10" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="57"/>
       <c r="D10" s="57"/>
@@ -3855,17 +3866,17 @@
       <c r="B2" s="55"/>
       <c r="C2" s="55"/>
       <c r="D2" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="55"/>
       <c r="C3" s="55"/>
       <c r="D3" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2">
         <f>H8</f>
@@ -3876,7 +3887,7 @@
       <c r="B4" s="55"/>
       <c r="C4" s="55"/>
       <c r="D4" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2">
         <f>I8</f>
@@ -3885,26 +3896,26 @@
     </row>
     <row r="6" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="37" t="s">
-        <v>65</v>
-      </c>
       <c r="I6" s="43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -3912,16 +3923,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="14">
         <v>18</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" s="20">
         <v>1400000</v>
@@ -3937,7 +3948,7 @@
     </row>
     <row r="8" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="57"/>
       <c r="D8" s="57"/>

</xml_diff>